<commit_message>
Cambios login, HU 3229, HU 3232 y avances HU 3233
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/DATA_VISOR_MOVISTAR.xlsx
+++ b/src/test/resources/excel/DATA_VISOR_MOVISTAR.xlsx
@@ -673,271 +673,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101005895DB48FFC38948ABBBD4F60E6523B9" ma:contentTypeVersion="16" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="d209d925d826d9b41c4a7a65aca2cf82">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="b1a116d1-37ca-478c-b0e0-036c2f54c177" xmlns:ns3="51bfb0fa-35ae-4a66-b3d4-c4ecfc995464" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bf53bca0ca86ae28f83ee0b23c68f9d6" ns1:_="" ns2:_="" ns3:_="">
-    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
-    <xsd:import namespace="b1a116d1-37ca-478c-b0e0-036c2f54c177"/>
-    <xsd:import namespace="51bfb0fa-35ae-4a66-b3d4-c4ecfc995464"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:Descripci_x00f3_n"/>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
-                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="13" nillable="true" ma:displayName="Propiedades de la Directiva de cumplimiento unificado" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="14" nillable="true" ma:displayName="Acción de IU de la Directiva de cumplimiento unificado" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b1a116d1-37ca-478c-b0e0-036c2f54c177" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="Descripci_x00f3_n" ma:index="2" ma:displayName="Descripción" ma:description="Breve descripción del archivo registrado" ma:internalName="Descripci_x00f3_n" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="15" nillable="true" ma:displayName="Tags" ma:hidden="true" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:hidden="true" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="19" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="20" nillable="true" ma:displayName="KeyPoints" ma:hidden="true" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="22" nillable="true" ma:displayName="Length (seconds)" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="51bfb0fa-35ae-4a66-b3d4-c4ecfc995464" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Compartido con" ma:hidden="true" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Detalles de uso compartido" ma:hidden="true" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:displayName="Tipo de contenido"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Título"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Descripci_x00f3_n xmlns="b1a116d1-37ca-478c-b0e0-036c2f54c177"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{965F58B7-93C8-42F7-B942-94E7891E56D9}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE62CB52-31CA-4EA0-9D56-5CFDB68F8DB5}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1741ADCD-1761-478C-AAD5-B1654041ED36}"/>
 </file>
</xml_diff>